<commit_message>
Updated 36 and 37
</commit_message>
<xml_diff>
--- a/Report_backlog_and_teamsheet.xlsx
+++ b/Report_backlog_and_teamsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\homework\SSW555\SSW-555-A-Project-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yikanwang/Documents/Spring2021/SSW555/SSW-555-A-Project-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B961B8-ED80-4B5E-AF52-A551344652B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693E3619-507B-224B-96B8-7777C7B58D15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,26 @@
     <sheet name="Sprint2" sheetId="7" r:id="rId5"/>
     <sheet name="Sprint3" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="230">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -526,7 +535,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -849,20 +858,35 @@
     <t>Compare every two brith date in the sorted list</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>US36</t>
+  </si>
+  <si>
+    <t>US37</t>
+  </si>
+  <si>
+    <t>Listdeath</t>
+  </si>
+  <si>
+    <t>list survivors</t>
+  </si>
+  <si>
+    <t>changed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -874,7 +898,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -888,14 +912,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -903,14 +927,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0066CC"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -924,7 +948,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -944,7 +968,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -953,7 +977,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -961,7 +985,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -969,14 +993,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1021,18 +1045,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1040,6 +1064,11 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1064,17 +1093,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{0806C502-5B25-4AE5-A7E3-7A9818F2DFE2}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="3" xr:uid="{5DC2A9AA-D403-45BD-9AB9-75B92DFC8BB2}"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1092,7 +1116,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1532,13 +1556,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1572,7 +1596,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1589,7 +1613,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1606,7 +1630,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1623,7 +1647,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1645,20 +1669,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C06F4B-E189-4612-9398-61FC56C851BF}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.109375" style="34" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="24" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1675,11 +1699,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C2" t="s">
@@ -1692,11 +1716,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C3" t="s">
@@ -1709,11 +1733,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
@@ -1726,11 +1750,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="24" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
@@ -1743,11 +1767,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
@@ -1760,11 +1784,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="24" t="s">
         <v>38</v>
       </c>
       <c r="C7" t="s">
@@ -1777,11 +1801,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="24" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
@@ -1794,11 +1818,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="24" t="s">
         <v>150</v>
       </c>
       <c r="C9" t="s">
@@ -1811,11 +1835,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>1</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="24" t="s">
         <v>152</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -1828,11 +1852,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>1</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="24" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1845,14 +1869,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="24" t="s">
         <v>154</v>
       </c>
       <c r="C13" t="s">
@@ -1865,11 +1889,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="24" t="s">
         <v>155</v>
       </c>
       <c r="C14" t="s">
@@ -1882,11 +1906,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="24" t="s">
         <v>138</v>
       </c>
       <c r="C15" t="s">
@@ -1899,11 +1923,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="24" t="s">
         <v>100</v>
       </c>
       <c r="C16" t="s">
@@ -1916,11 +1940,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="24" t="s">
         <v>158</v>
       </c>
       <c r="C17" t="s">
@@ -1933,11 +1957,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="24" t="s">
         <v>161</v>
       </c>
       <c r="C18" t="s">
@@ -1950,11 +1974,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="24" t="s">
         <v>145</v>
       </c>
       <c r="C19" t="s">
@@ -1967,11 +1991,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="24" t="s">
         <v>147</v>
       </c>
       <c r="C20" t="s">
@@ -1984,11 +2008,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="16">
         <v>2</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C21" s="16" t="s">
@@ -2001,11 +2025,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
         <v>2</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="24" t="s">
         <v>143</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -2018,11 +2042,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>3</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="25" t="s">
         <v>164</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -2032,14 +2056,14 @@
         <v>166</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>3</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="25" t="s">
         <v>167</v>
       </c>
       <c r="C25" s="20" t="s">
@@ -2049,14 +2073,14 @@
         <v>166</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="24" t="s">
         <v>192</v>
       </c>
       <c r="C26" t="s">
@@ -2069,11 +2093,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="24" t="s">
         <v>176</v>
       </c>
       <c r="C27" t="s">
@@ -2086,11 +2110,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="24" t="s">
         <v>190</v>
       </c>
       <c r="C28" t="s">
@@ -2103,11 +2127,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>3</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="24" t="s">
         <v>186</v>
       </c>
       <c r="C29" s="22" t="s">
@@ -2120,11 +2144,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="24" t="s">
         <v>206</v>
       </c>
       <c r="C30" s="23" t="s">
@@ -2137,11 +2161,11 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="24" t="s">
         <v>207</v>
       </c>
       <c r="C31" s="23" t="s">
@@ -2152,6 +2176,40 @@
       </c>
       <c r="E31" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" t="s">
+        <v>227</v>
+      </c>
+      <c r="D32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="C33" t="s">
+        <v>228</v>
+      </c>
+      <c r="D33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2172,19 +2230,19 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="8"/>
-    <col min="2" max="2" width="20.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="8"/>
+    <col min="2" max="2" width="20.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="8" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="8" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="12.44140625" style="8"/>
+    <col min="8" max="16384" width="12.5" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>139</v>
       </c>
@@ -2207,7 +2265,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>140</v>
       </c>
@@ -2221,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="13">
         <v>44273</v>
       </c>
@@ -2244,7 +2302,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="18">
         <v>44277</v>
       </c>
@@ -2265,7 +2323,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>141</v>
       </c>
@@ -2289,7 +2347,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>178</v>
       </c>
@@ -2319,20 +2377,20 @@
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.88671875" customWidth="1"/>
+    <col min="13" max="13" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2361,7 +2419,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2389,20 +2447,20 @@
       <c r="I2" s="15">
         <v>44272</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K3" s="29" t="s">
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K3" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -2412,13 +2470,13 @@
       <c r="C4" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -2428,13 +2486,13 @@
       <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+    </row>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2444,16 +2502,16 @@
       <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2478,20 +2536,20 @@
       <c r="I8" s="15">
         <v>44272</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K9" s="24" t="s">
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K9" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+    </row>
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2504,13 +2562,13 @@
       <c r="D10" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+    </row>
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2521,7 +2579,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2532,14 +2590,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K13" s="25" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K13" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+    </row>
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2567,14 +2625,14 @@
       <c r="I14" s="15">
         <v>44258</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="31">
         <f>SUM(H:H)</f>
         <v>230</v>
       </c>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2588,7 +2646,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -2602,7 +2660,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -2631,7 +2689,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -2645,7 +2703,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -2659,7 +2717,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2679,7 +2737,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -2708,7 +2766,7 @@
         <v>44282</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -2729,7 +2787,7 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -2738,7 +2796,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>73</v>
       </c>
@@ -2755,7 +2813,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>74</v>
       </c>
@@ -2772,7 +2830,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>74</v>
       </c>
@@ -2787,7 +2845,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -2796,7 +2854,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>31</v>
       </c>
@@ -2817,7 +2875,7 @@
       </c>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -2826,7 +2884,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>89</v>
       </c>
@@ -2841,7 +2899,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>91</v>
       </c>
@@ -2856,7 +2914,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>92</v>
       </c>
@@ -2899,14 +2957,14 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="57.109375" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="16" max="16" width="32.109375" customWidth="1"/>
+    <col min="16" max="16" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
@@ -2935,7 +2993,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -2963,23 +3021,23 @@
       <c r="I2" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K3" s="29" t="s">
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K3" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -2989,16 +3047,16 @@
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -3008,16 +3066,16 @@
       <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -3028,7 +3086,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -3039,17 +3097,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K8" s="31" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K8" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -3077,26 +3135,26 @@
       <c r="I9" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K10" s="30" t="s">
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K10" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>173</v>
       </c>
@@ -3107,7 +3165,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -3118,7 +3176,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>175</v>
       </c>
@@ -3128,24 +3186,24 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="K13" s="31" t="s">
+      <c r="K13" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>98</v>
       </c>
@@ -3172,7 +3230,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -3183,7 +3241,7 @@
       <c r="H16" s="16"/>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>105</v>
       </c>
@@ -3200,7 +3258,7 @@
       <c r="H17" s="16"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -3211,7 +3269,7 @@
       <c r="H18" s="16"/>
       <c r="I18" s="15"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -3222,7 +3280,7 @@
       <c r="H19" s="16"/>
       <c r="I19" s="15"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>100</v>
       </c>
@@ -3249,7 +3307,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -3260,7 +3318,7 @@
       <c r="H21" s="16"/>
       <c r="I21" s="15"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
@@ -3277,7 +3335,7 @@
       <c r="H22" s="16"/>
       <c r="I22" s="15"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -3288,7 +3346,7 @@
       <c r="H23" s="16"/>
       <c r="I23" s="15"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>144</v>
       </c>
@@ -3313,7 +3371,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>146</v>
       </c>
@@ -3363,13 +3421,13 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="53.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="53.5" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
@@ -3398,7 +3456,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -3427,7 +3485,7 @@
         <v>44299</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -3438,7 +3496,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -3449,7 +3507,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>183</v>
       </c>
@@ -3460,7 +3518,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>186</v>
       </c>
@@ -3489,7 +3547,7 @@
         <v>44299</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>184</v>
       </c>
@@ -3500,7 +3558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>185</v>
       </c>
@@ -3511,7 +3569,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>190</v>
       </c>
@@ -3540,7 +3598,7 @@
         <v>44299</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -3551,7 +3609,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>195</v>
       </c>
@@ -3568,7 +3626,7 @@
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>196</v>
       </c>
@@ -3585,7 +3643,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>192</v>
       </c>
@@ -3614,7 +3672,7 @@
         <v>44299</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -3625,7 +3683,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>198</v>
       </c>
@@ -3642,7 +3700,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>199</v>
       </c>
@@ -3659,11 +3717,11 @@
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="27" t="s">
         <v>202</v>
       </c>
       <c r="C25" t="s">
@@ -3684,11 +3742,11 @@
       <c r="H25">
         <v>120</v>
       </c>
-      <c r="I25" s="36">
+      <c r="I25" s="26">
         <v>44301</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>211</v>
       </c>
@@ -3699,7 +3757,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
         <v>212</v>
       </c>
@@ -3710,7 +3768,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>213</v>
       </c>
@@ -3721,11 +3779,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="28" t="s">
         <v>205</v>
       </c>
       <c r="C31" s="23" t="s">
@@ -3746,11 +3804,11 @@
       <c r="H31">
         <v>100</v>
       </c>
-      <c r="I31" s="36">
+      <c r="I31" s="26">
         <v>44301</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>217</v>
       </c>
@@ -3761,7 +3819,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>218</v>
       </c>
@@ -3772,7 +3830,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>222</v>
       </c>
@@ -3783,7 +3841,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
         <v>223</v>
       </c>

</xml_diff>